<commit_message>
Update report-Steel Plate Defect Prediction.xlsx
</commit_message>
<xml_diff>
--- a/Steel Plate Defect Prediction/report-Steel Plate Defect Prediction.xlsx
+++ b/Steel Plate Defect Prediction/report-Steel Plate Defect Prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darab Store\Desktop\ML-projects\Git-Hub\PlayGround-Competition\Steel Plate Defect Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C3B8C9D-2354-4096-979D-66175B7414E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E2DB9A-2C2F-46AB-8940-086D722324E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,31 +169,31 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -479,292 +479,336 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D10"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.5">
       <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4" t="s">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="4"/>
+      <c r="Q1" s="9"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="P11:P13"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="N11:N13"/>
-    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="O5:O7"/>
     <mergeCell ref="P8:P10"/>
     <mergeCell ref="Q8:Q10"/>
     <mergeCell ref="B11:B13"/>
@@ -781,58 +825,14 @@
     <mergeCell ref="M8:M10"/>
     <mergeCell ref="N8:N10"/>
     <mergeCell ref="O8:O10"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="Q5:Q7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="P11:P13"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="N11:N13"/>
+    <mergeCell ref="O11:O13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>